<commit_message>
feat: Binding List by reading excel file in Import function
</commit_message>
<xml_diff>
--- a/BookStore.xlsx
+++ b/BookStore.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\3rd\HK2\LTWD\Implements\Project_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\3rd\HK2\LTWD\Implements\Project_1\CKDP-College-Book-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FDBA031-2BD5-4F81-85B5-637C1C457BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE35CD4D-9D42-4975-A036-1E4F2BFA182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{448C2645-1BD2-4265-8D27-E94F11A4866E}"/>
   </bookViews>
@@ -294,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -309,12 +309,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,7 +631,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +640,7 @@
     <col min="2" max="2" width="31.5546875" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="22.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
@@ -658,7 +657,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -678,7 +677,7 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>2023</v>
       </c>
       <c r="F2" s="2">
@@ -698,7 +697,7 @@
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>2022</v>
       </c>
       <c r="F3" s="2">
@@ -1018,7 +1017,7 @@
       <c r="D19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>2002</v>
       </c>
       <c r="F19" s="2">
@@ -1038,7 +1037,7 @@
       <c r="D20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>2010</v>
       </c>
       <c r="F20" s="2">
@@ -1058,7 +1057,7 @@
       <c r="D21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>2008</v>
       </c>
       <c r="F21" s="2">
@@ -1078,7 +1077,7 @@
       <c r="D22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>2001</v>
       </c>
       <c r="F22" s="2">
@@ -1098,7 +1097,7 @@
       <c r="D23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>2012</v>
       </c>
       <c r="F23" s="2">
@@ -1118,7 +1117,7 @@
       <c r="D24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>2020</v>
       </c>
       <c r="F24" s="2">
@@ -1138,7 +1137,7 @@
       <c r="D25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>2020</v>
       </c>
       <c r="F25" s="2">
@@ -1158,7 +1157,7 @@
       <c r="D26" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>2019</v>
       </c>
       <c r="F26" s="2">
@@ -1178,7 +1177,7 @@
       <c r="D27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>2017</v>
       </c>
       <c r="F27" s="2">
@@ -1198,7 +1197,7 @@
       <c r="D28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>2008</v>
       </c>
       <c r="F28" s="2">
@@ -1218,7 +1217,7 @@
       <c r="D29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>2010</v>
       </c>
       <c r="F29" s="2">
@@ -1238,7 +1237,7 @@
       <c r="D30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>2021</v>
       </c>
       <c r="F30" s="2">
@@ -1258,7 +1257,7 @@
       <c r="D31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>2023</v>
       </c>
       <c r="F31" s="2">
@@ -1281,7 +1280,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.21875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: Binding Categories in Dashboard Ribbon by reading Excel file in Import funtion, display Price of Books
</commit_message>
<xml_diff>
--- a/BookStore.xlsx
+++ b/BookStore.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\3rd\HK2\LTWD\Implements\Project_1\CKDP-College-Book-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE35CD4D-9D42-4975-A036-1E4F2BFA182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00BB2F1-7306-4549-96FA-19215623C8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{448C2645-1BD2-4265-8D27-E94F11A4866E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{448C2645-1BD2-4265-8D27-E94F11A4866E}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
-    <sheet name="TypeOfProduct" sheetId="2" r:id="rId2"/>
+    <sheet name="Category" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>ID</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Academic</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -294,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -314,6 +317,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49FDE29-0A55-4969-B922-367A4B725963}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,10 +647,10 @@
     <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="22.77734375" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="6" max="7" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -663,8 +669,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -683,8 +692,11 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="2">
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -703,8 +715,11 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="2">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -723,8 +738,11 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -743,8 +761,11 @@
       <c r="F5" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="2">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -763,8 +784,11 @@
       <c r="F6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="2">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -783,8 +807,11 @@
       <c r="F7" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -803,8 +830,11 @@
       <c r="F8" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="2">
+        <v>700000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -823,8 +853,12 @@
       <c r="F9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="2">
+        <v>100000</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -843,8 +877,12 @@
       <c r="F10" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="2">
+        <v>70000</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -863,8 +901,12 @@
       <c r="F11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="2">
+        <v>3000000</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -883,8 +925,12 @@
       <c r="F12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="2">
+        <v>200000</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -903,8 +949,12 @@
       <c r="F13" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="2">
+        <v>4000000</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -923,8 +973,12 @@
       <c r="F14" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="2">
+        <v>60000</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -943,8 +997,12 @@
       <c r="F15" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="2">
+        <v>200000</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -963,8 +1021,12 @@
       <c r="F16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="2">
+        <v>20000</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -983,8 +1045,12 @@
       <c r="F17" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="2">
+        <v>80000</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1003,8 +1069,12 @@
       <c r="F18" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1023,8 +1093,12 @@
       <c r="F19" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1043,8 +1117,12 @@
       <c r="F20" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="2">
+        <v>100000</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1063,8 +1141,12 @@
       <c r="F21" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="2">
+        <v>30000</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1083,8 +1165,12 @@
       <c r="F22" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="2">
+        <v>200000</v>
+      </c>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1103,8 +1189,12 @@
       <c r="F23" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="2">
+        <v>60000</v>
+      </c>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1123,8 +1213,12 @@
       <c r="F24" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1143,8 +1237,12 @@
       <c r="F25" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="2">
+        <v>200000</v>
+      </c>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1163,8 +1261,12 @@
       <c r="F26" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="2">
+        <v>70000</v>
+      </c>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1183,8 +1285,12 @@
       <c r="F27" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="2">
+        <v>40000</v>
+      </c>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1203,8 +1309,12 @@
       <c r="F28" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="2">
+        <v>6000000</v>
+      </c>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1223,8 +1333,12 @@
       <c r="F29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1243,8 +1357,12 @@
       <c r="F30" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="2">
+        <v>100000</v>
+      </c>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>35</v>
       </c>
@@ -1263,6 +1381,31 @@
       <c r="F31" s="2">
         <v>5</v>
       </c>
+      <c r="G31" s="2">
+        <v>60000</v>
+      </c>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J38" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1274,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE1C845-C091-4F14-87C2-D4D11FE1EF8E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: Creat DBContext Class and connect to db to write data from file when importing
</commit_message>
<xml_diff>
--- a/BookStore.xlsx
+++ b/BookStore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\3rd\HK2\LTWD\Implements\Project_1\CKDP-College-Book-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00BB2F1-7306-4549-96FA-19215623C8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD51512-8887-415E-AD79-0471E20184E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{448C2645-1BD2-4265-8D27-E94F11A4866E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{448C2645-1BD2-4265-8D27-E94F11A4866E}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>Raw Price</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -320,6 +326,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49FDE29-0A55-4969-B922-367A4B725963}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,10 +655,11 @@
     <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="22.77734375" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" style="8" customWidth="1"/>
-    <col min="6" max="7" width="8.88671875" style="4"/>
+    <col min="6" max="6" width="10.44140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -667,13 +676,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H1" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -695,8 +707,11 @@
       <c r="G2" s="2">
         <v>900000</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H2" s="1">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -718,8 +733,11 @@
       <c r="G3" s="2">
         <v>5000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="1">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -741,8 +759,11 @@
       <c r="G4" s="2">
         <v>600000</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H4" s="1">
+        <v>480000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -764,8 +785,11 @@
       <c r="G5" s="2">
         <v>60000</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H5" s="1">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -787,8 +811,12 @@
       <c r="G6" s="2">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H6" s="1">
+        <v>1600000</v>
+      </c>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -810,8 +838,12 @@
       <c r="G7" s="2">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H7" s="1">
+        <v>8000000</v>
+      </c>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -833,8 +865,12 @@
       <c r="G8" s="2">
         <v>700000</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H8" s="1">
+        <v>560000</v>
+      </c>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -856,9 +892,13 @@
       <c r="G9" s="2">
         <v>100000</v>
       </c>
+      <c r="H9" s="1">
+        <v>80000</v>
+      </c>
       <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -880,9 +920,13 @@
       <c r="G10" s="2">
         <v>70000</v>
       </c>
+      <c r="H10" s="1">
+        <v>56000</v>
+      </c>
       <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -904,9 +948,13 @@
       <c r="G11" s="2">
         <v>3000000</v>
       </c>
+      <c r="H11" s="1">
+        <v>2400000</v>
+      </c>
       <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -928,9 +976,13 @@
       <c r="G12" s="2">
         <v>200000</v>
       </c>
+      <c r="H12" s="1">
+        <v>160000</v>
+      </c>
       <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -952,9 +1004,13 @@
       <c r="G13" s="2">
         <v>4000000</v>
       </c>
+      <c r="H13" s="1">
+        <v>3200000</v>
+      </c>
       <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -976,9 +1032,13 @@
       <c r="G14" s="2">
         <v>60000</v>
       </c>
+      <c r="H14" s="1">
+        <v>48000</v>
+      </c>
       <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1000,9 +1060,13 @@
       <c r="G15" s="2">
         <v>200000</v>
       </c>
+      <c r="H15" s="1">
+        <v>160000</v>
+      </c>
       <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1024,9 +1088,13 @@
       <c r="G16" s="2">
         <v>20000</v>
       </c>
+      <c r="H16" s="1">
+        <v>16000</v>
+      </c>
       <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1048,9 +1116,13 @@
       <c r="G17" s="2">
         <v>80000</v>
       </c>
+      <c r="H17" s="1">
+        <v>64000</v>
+      </c>
       <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1072,9 +1144,13 @@
       <c r="G18" s="2">
         <v>10000</v>
       </c>
+      <c r="H18" s="1">
+        <v>8000</v>
+      </c>
       <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1096,9 +1172,13 @@
       <c r="G19" s="2">
         <v>1000000</v>
       </c>
+      <c r="H19" s="1">
+        <v>800000</v>
+      </c>
       <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1120,9 +1200,13 @@
       <c r="G20" s="2">
         <v>100000</v>
       </c>
+      <c r="H20" s="1">
+        <v>80000</v>
+      </c>
       <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1144,9 +1228,13 @@
       <c r="G21" s="2">
         <v>30000</v>
       </c>
+      <c r="H21" s="1">
+        <v>24000</v>
+      </c>
       <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1168,9 +1256,13 @@
       <c r="G22" s="2">
         <v>200000</v>
       </c>
+      <c r="H22" s="1">
+        <v>160000</v>
+      </c>
       <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L22" s="11"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1192,9 +1284,13 @@
       <c r="G23" s="2">
         <v>60000</v>
       </c>
+      <c r="H23" s="1">
+        <v>48000</v>
+      </c>
       <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1216,9 +1312,13 @@
       <c r="G24" s="2">
         <v>1000000</v>
       </c>
+      <c r="H24" s="1">
+        <v>800000</v>
+      </c>
       <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1240,9 +1340,13 @@
       <c r="G25" s="2">
         <v>200000</v>
       </c>
+      <c r="H25" s="1">
+        <v>160000</v>
+      </c>
       <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1264,9 +1368,13 @@
       <c r="G26" s="2">
         <v>70000</v>
       </c>
+      <c r="H26" s="1">
+        <v>56000</v>
+      </c>
       <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L26" s="11"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1288,9 +1396,13 @@
       <c r="G27" s="2">
         <v>40000</v>
       </c>
+      <c r="H27" s="1">
+        <v>32000</v>
+      </c>
       <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L27" s="11"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1312,9 +1424,13 @@
       <c r="G28" s="2">
         <v>6000000</v>
       </c>
+      <c r="H28" s="1">
+        <v>4800000</v>
+      </c>
       <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L28" s="11"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1336,9 +1452,13 @@
       <c r="G29" s="2">
         <v>1000000</v>
       </c>
+      <c r="H29" s="1">
+        <v>800000</v>
+      </c>
       <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L29" s="11"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1360,9 +1480,13 @@
       <c r="G30" s="2">
         <v>100000</v>
       </c>
+      <c r="H30" s="1">
+        <v>80000</v>
+      </c>
       <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L30" s="11"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>35</v>
       </c>
@@ -1384,27 +1508,36 @@
       <c r="G31" s="2">
         <v>60000</v>
       </c>
+      <c r="H31" s="1">
+        <v>48000</v>
+      </c>
       <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L31" s="11"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="L32" s="11"/>
+    </row>
+    <row r="33" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="L33" s="11"/>
+    </row>
+    <row r="34" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="L34" s="11"/>
+    </row>
+    <row r="35" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="L35" s="11"/>
+    </row>
+    <row r="36" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="L36" s="11"/>
+    </row>
+    <row r="37" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J38" s="4"/>
     </row>
   </sheetData>
@@ -1417,7 +1550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE1C845-C091-4F14-87C2-D4D11FE1EF8E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: Obfuscator and Deploy app
</commit_message>
<xml_diff>
--- a/BookStore.xlsx
+++ b/BookStore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\3rd\HK2\LTWD\Implements\Project_1\CKDP-College-Book-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD51512-8887-415E-AD79-0471E20184E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85692362-C1B1-4BA8-B0D6-26960FFBFB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{448C2645-1BD2-4265-8D27-E94F11A4866E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -225,12 +225,6 @@
     <t>Dám thất bại</t>
   </si>
   <si>
-    <t>Cach ket noi database</t>
-  </si>
-  <si>
-    <t>Tran Duy Quang</t>
-  </si>
-  <si>
     <t>Novel</t>
   </si>
   <si>
@@ -253,6 +247,105 @@
   </si>
   <si>
     <t>Raw Price</t>
+  </si>
+  <si>
+    <t>Images/2.jpg</t>
+  </si>
+  <si>
+    <t>Images/3.jpg</t>
+  </si>
+  <si>
+    <t>Images/4.jpg</t>
+  </si>
+  <si>
+    <t>Images/5.jpg</t>
+  </si>
+  <si>
+    <t>Images/6.jpg</t>
+  </si>
+  <si>
+    <t>Images/7.jpg</t>
+  </si>
+  <si>
+    <t>Images/8.jpg</t>
+  </si>
+  <si>
+    <t>Images/9.jpg</t>
+  </si>
+  <si>
+    <t>Images/10.jpg</t>
+  </si>
+  <si>
+    <t>Images/11.jpg</t>
+  </si>
+  <si>
+    <t>Images/12.jpg</t>
+  </si>
+  <si>
+    <t>Images/13.jpg</t>
+  </si>
+  <si>
+    <t>Images/14.jpg</t>
+  </si>
+  <si>
+    <t>Images/15.jpg</t>
+  </si>
+  <si>
+    <t>Images/16.jpg</t>
+  </si>
+  <si>
+    <t>Images/17.jpg</t>
+  </si>
+  <si>
+    <t>Images/18.jpg</t>
+  </si>
+  <si>
+    <t>Images/19.jpg</t>
+  </si>
+  <si>
+    <t>Images/20.jpg</t>
+  </si>
+  <si>
+    <t>Images/21.jpg</t>
+  </si>
+  <si>
+    <t>Images/22.jpg</t>
+  </si>
+  <si>
+    <t>Images/23.jpg</t>
+  </si>
+  <si>
+    <t>Images/24.jpg</t>
+  </si>
+  <si>
+    <t>Images/25.jpg</t>
+  </si>
+  <si>
+    <t>Images/26.jpg</t>
+  </si>
+  <si>
+    <t>Images/27.jpg</t>
+  </si>
+  <si>
+    <t>Images/28.jpg</t>
+  </si>
+  <si>
+    <t>Images/29.jpg</t>
+  </si>
+  <si>
+    <t>Billi P.S. Lim</t>
+  </si>
+  <si>
+    <t>Nhà giả kim</t>
+  </si>
+  <si>
+    <t>Images/30.jpg</t>
+  </si>
+  <si>
+    <t>Paulo Coelho</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -326,8 +419,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49FDE29-0A55-4969-B922-367A4B725963}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,10 +748,11 @@
     <col min="1" max="1" width="5.21875" style="4" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12" style="4" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="4"/>
+    <col min="9" max="9" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -666,23 +762,26 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>72</v>
+      <c r="I1" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -695,10 +794,10 @@
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>2023</v>
       </c>
       <c r="F2" s="2">
@@ -709,6 +808,9 @@
       </c>
       <c r="H2" s="1">
         <v>720000</v>
+      </c>
+      <c r="I2" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -719,12 +821,12 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>2022</v>
       </c>
       <c r="F3" s="2">
@@ -735,6 +837,9 @@
       </c>
       <c r="H3" s="1">
         <v>4000000</v>
+      </c>
+      <c r="I3" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -745,12 +850,12 @@
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>2022</v>
       </c>
       <c r="F4" s="2">
@@ -761,6 +866,9 @@
       </c>
       <c r="H4" s="1">
         <v>480000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -771,12 +879,12 @@
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>2014</v>
       </c>
       <c r="F5" s="2">
@@ -788,6 +896,10 @@
       <c r="H5" s="1">
         <v>48000</v>
       </c>
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -797,12 +909,12 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>2022</v>
       </c>
       <c r="F6" s="2">
@@ -814,7 +926,10 @@
       <c r="H6" s="1">
         <v>1600000</v>
       </c>
-      <c r="L6" s="11"/>
+      <c r="I6" s="2">
+        <v>12</v>
+      </c>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -824,12 +939,12 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>2011</v>
       </c>
       <c r="F7" s="2">
@@ -841,7 +956,10 @@
       <c r="H7" s="1">
         <v>8000000</v>
       </c>
-      <c r="L7" s="11"/>
+      <c r="I7" s="2">
+        <v>13</v>
+      </c>
+      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -851,12 +969,12 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>2017</v>
       </c>
       <c r="F8" s="2">
@@ -868,7 +986,11 @@
       <c r="H8" s="1">
         <v>560000</v>
       </c>
-      <c r="L8" s="11"/>
+      <c r="I8" s="2">
+        <v>10</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -878,12 +1000,12 @@
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>2010</v>
       </c>
       <c r="F9" s="2">
@@ -895,8 +1017,11 @@
       <c r="H9" s="1">
         <v>80000</v>
       </c>
+      <c r="I9" s="2">
+        <v>7</v>
+      </c>
       <c r="J9" s="4"/>
-      <c r="L9" s="11"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -906,12 +1031,12 @@
         <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>2022</v>
       </c>
       <c r="F10" s="2">
@@ -923,8 +1048,11 @@
       <c r="H10" s="1">
         <v>56000</v>
       </c>
+      <c r="I10" s="2">
+        <v>9</v>
+      </c>
       <c r="J10" s="4"/>
-      <c r="L10" s="11"/>
+      <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -934,12 +1062,12 @@
         <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>2022</v>
       </c>
       <c r="F11" s="2">
@@ -951,8 +1079,11 @@
       <c r="H11" s="1">
         <v>2400000</v>
       </c>
+      <c r="I11" s="2">
+        <v>2</v>
+      </c>
       <c r="J11" s="4"/>
-      <c r="L11" s="11"/>
+      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -962,12 +1093,12 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>2022</v>
       </c>
       <c r="F12" s="2">
@@ -979,8 +1110,11 @@
       <c r="H12" s="1">
         <v>160000</v>
       </c>
+      <c r="I12" s="2">
+        <v>4</v>
+      </c>
       <c r="J12" s="4"/>
-      <c r="L12" s="11"/>
+      <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
@@ -990,12 +1124,12 @@
         <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>2012</v>
       </c>
       <c r="F13" s="2">
@@ -1007,8 +1141,11 @@
       <c r="H13" s="1">
         <v>3200000</v>
       </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
       <c r="J13" s="4"/>
-      <c r="L13" s="11"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
@@ -1018,12 +1155,12 @@
         <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>2020</v>
       </c>
       <c r="F14" s="2">
@@ -1035,8 +1172,11 @@
       <c r="H14" s="1">
         <v>48000</v>
       </c>
+      <c r="I14" s="2">
+        <v>8</v>
+      </c>
       <c r="J14" s="4"/>
-      <c r="L14" s="11"/>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
@@ -1046,12 +1186,12 @@
         <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="3">
         <v>2023</v>
       </c>
       <c r="F15" s="2">
@@ -1063,8 +1203,11 @@
       <c r="H15" s="1">
         <v>160000</v>
       </c>
+      <c r="I15" s="2">
+        <v>6</v>
+      </c>
       <c r="J15" s="4"/>
-      <c r="L15" s="11"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -1074,12 +1217,12 @@
         <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="3">
         <v>2023</v>
       </c>
       <c r="F16" s="2">
@@ -1091,8 +1234,11 @@
       <c r="H16" s="1">
         <v>16000</v>
       </c>
+      <c r="I16" s="2">
+        <v>3</v>
+      </c>
       <c r="J16" s="4"/>
-      <c r="L16" s="11"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
@@ -1102,12 +1248,12 @@
         <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="3">
         <v>2022</v>
       </c>
       <c r="F17" s="2">
@@ -1119,8 +1265,11 @@
       <c r="H17" s="1">
         <v>64000</v>
       </c>
+      <c r="I17" s="2">
+        <v>3</v>
+      </c>
       <c r="J17" s="4"/>
-      <c r="L17" s="11"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
@@ -1130,12 +1279,12 @@
         <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="3">
         <v>2010</v>
       </c>
       <c r="F18" s="2">
@@ -1147,8 +1296,11 @@
       <c r="H18" s="1">
         <v>8000</v>
       </c>
+      <c r="I18" s="2">
+        <v>7</v>
+      </c>
       <c r="J18" s="4"/>
-      <c r="L18" s="11"/>
+      <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
@@ -1158,12 +1310,12 @@
         <v>41</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="3">
         <v>2002</v>
       </c>
       <c r="F19" s="2">
@@ -1175,8 +1327,11 @@
       <c r="H19" s="1">
         <v>800000</v>
       </c>
+      <c r="I19" s="2">
+        <v>15</v>
+      </c>
       <c r="J19" s="4"/>
-      <c r="L19" s="11"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
@@ -1186,12 +1341,12 @@
         <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="3">
         <v>2010</v>
       </c>
       <c r="F20" s="2">
@@ -1203,8 +1358,11 @@
       <c r="H20" s="1">
         <v>80000</v>
       </c>
+      <c r="I20" s="2">
+        <v>11</v>
+      </c>
       <c r="J20" s="4"/>
-      <c r="L20" s="11"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
@@ -1214,12 +1372,12 @@
         <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="3">
         <v>2008</v>
       </c>
       <c r="F21" s="2">
@@ -1231,8 +1389,11 @@
       <c r="H21" s="1">
         <v>24000</v>
       </c>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
       <c r="J21" s="4"/>
-      <c r="L21" s="11"/>
+      <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
@@ -1242,12 +1403,12 @@
         <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="3">
         <v>2001</v>
       </c>
       <c r="F22" s="2">
@@ -1259,8 +1420,11 @@
       <c r="H22" s="1">
         <v>160000</v>
       </c>
+      <c r="I22" s="2">
+        <v>4</v>
+      </c>
       <c r="J22" s="4"/>
-      <c r="L22" s="11"/>
+      <c r="L22" s="10"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
@@ -1270,12 +1434,12 @@
         <v>48</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="3">
         <v>2012</v>
       </c>
       <c r="F23" s="2">
@@ -1287,8 +1451,11 @@
       <c r="H23" s="1">
         <v>48000</v>
       </c>
+      <c r="I23" s="2">
+        <v>3</v>
+      </c>
       <c r="J23" s="4"/>
-      <c r="L23" s="11"/>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
@@ -1298,12 +1465,12 @@
         <v>50</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="3">
         <v>2020</v>
       </c>
       <c r="F24" s="2">
@@ -1315,8 +1482,11 @@
       <c r="H24" s="1">
         <v>800000</v>
       </c>
+      <c r="I24" s="2">
+        <v>8</v>
+      </c>
       <c r="J24" s="4"/>
-      <c r="L24" s="11"/>
+      <c r="L24" s="10"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
@@ -1326,12 +1496,12 @@
         <v>52</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="3">
         <v>2020</v>
       </c>
       <c r="F25" s="2">
@@ -1343,8 +1513,11 @@
       <c r="H25" s="1">
         <v>160000</v>
       </c>
+      <c r="I25" s="2">
+        <v>9</v>
+      </c>
       <c r="J25" s="4"/>
-      <c r="L25" s="11"/>
+      <c r="L25" s="10"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
@@ -1354,12 +1527,12 @@
         <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="3">
         <v>2019</v>
       </c>
       <c r="F26" s="2">
@@ -1371,8 +1544,10 @@
       <c r="H26" s="1">
         <v>56000</v>
       </c>
+      <c r="I26" s="2">
+        <v>7</v>
+      </c>
       <c r="J26" s="4"/>
-      <c r="L26" s="11"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
@@ -1382,12 +1557,12 @@
         <v>56</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="3">
         <v>2017</v>
       </c>
       <c r="F27" s="2">
@@ -1399,8 +1574,10 @@
       <c r="H27" s="1">
         <v>32000</v>
       </c>
+      <c r="I27" s="2">
+        <v>4</v>
+      </c>
       <c r="J27" s="4"/>
-      <c r="L27" s="11"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
@@ -1410,12 +1587,12 @@
         <v>58</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="3">
         <v>2008</v>
       </c>
       <c r="F28" s="2">
@@ -1427,8 +1604,10 @@
       <c r="H28" s="1">
         <v>4800000</v>
       </c>
+      <c r="I28" s="2">
+        <v>3</v>
+      </c>
       <c r="J28" s="4"/>
-      <c r="L28" s="11"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
@@ -1438,12 +1617,12 @@
         <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="3">
         <v>2010</v>
       </c>
       <c r="F29" s="2">
@@ -1455,8 +1634,10 @@
       <c r="H29" s="1">
         <v>800000</v>
       </c>
+      <c r="I29" s="2">
+        <v>2</v>
+      </c>
       <c r="J29" s="4"/>
-      <c r="L29" s="11"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
@@ -1466,12 +1647,12 @@
         <v>62</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="5">
+        <v>98</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="3">
         <v>2021</v>
       </c>
       <c r="F30" s="2">
@@ -1483,24 +1664,26 @@
       <c r="H30" s="1">
         <v>80000</v>
       </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
       <c r="J30" s="4"/>
-      <c r="L30" s="11"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>35</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="5">
-        <v>2023</v>
+      <c r="B31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1988</v>
       </c>
       <c r="F31" s="2">
         <v>5</v>
@@ -1511,34 +1694,28 @@
       <c r="H31" s="1">
         <v>48000</v>
       </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
       <c r="J31" s="4"/>
-      <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J32" s="4"/>
-      <c r="L32" s="11"/>
-    </row>
-    <row r="33" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J33" s="4"/>
-      <c r="L33" s="11"/>
-    </row>
-    <row r="34" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J34" s="4"/>
-      <c r="L34" s="11"/>
-    </row>
-    <row r="35" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J35" s="4"/>
-      <c r="L35" s="11"/>
-    </row>
-    <row r="36" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J36" s="4"/>
-      <c r="L36" s="11"/>
-    </row>
-    <row r="37" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J38" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1572,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1580,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1588,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1596,7 +1773,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1604,7 +1781,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>